<commit_message>
Added columns to summary
</commit_message>
<xml_diff>
--- a/Python/Data/Final/summary.xlsx
+++ b/Python/Data/Final/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\IUB\CNS_parttime\ASCTB Azimuth Comparison\ASCTB-Azimuth-Comparison-22\Python\Data\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3BA2B7-C61B-487B-92FF-F2942B68377E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF1208A-0F44-4B41-B1F2-6D24353DC4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Organ</t>
   </si>
@@ -34,16 +34,22 @@
     <t>Az_Asctb_perfect_matches</t>
   </si>
   <si>
+    <t>ASCTB_unique_CT</t>
+  </si>
+  <si>
+    <t>Azimuth_unique_CT</t>
+  </si>
+  <si>
     <t>Az_incorrect_cts</t>
   </si>
   <si>
     <t>Asctb_incorrect_cts</t>
   </si>
   <si>
-    <t>Az_match_found_corsswalk</t>
-  </si>
-  <si>
-    <t>Asctb_match_found_corsswalk</t>
+    <t>Az_ct_match_found_corsswalk</t>
+  </si>
+  <si>
+    <t>Asctb_ct_match_found_corsswalk</t>
   </si>
   <si>
     <t>Asctb_cts_mismatch_final</t>
@@ -472,27 +478,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" customWidth="1"/>
-    <col min="8" max="8" width="27.109375" customWidth="1"/>
-    <col min="9" max="9" width="24.21875" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="34.21875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="24.77734375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,10 +532,16 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -538,27 +553,33 @@
         <v>14</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2">
+        <v>43</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
         <v>31</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="2">
         <v>4</v>
       </c>
-      <c r="H2" s="2">
+      <c r="J2" s="2">
         <v>28</v>
       </c>
-      <c r="I2" s="2">
+      <c r="K2" s="2">
         <v>22</v>
       </c>
-      <c r="J2" s="2">
+      <c r="L2" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -570,27 +591,33 @@
         <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
         <v>5</v>
       </c>
-      <c r="I3" s="2">
+      <c r="K3" s="2">
         <v>12</v>
       </c>
-      <c r="J3" s="2">
+      <c r="L3" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -602,27 +629,33 @@
         <v>26</v>
       </c>
       <c r="E4" s="2">
+        <v>47</v>
+      </c>
+      <c r="F4" s="2">
+        <v>42</v>
+      </c>
+      <c r="G4" s="2">
         <v>7</v>
       </c>
-      <c r="F4" s="2">
+      <c r="H4" s="2">
         <v>12</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="2">
         <v>11</v>
       </c>
-      <c r="I4" s="2">
+      <c r="K4" s="2">
         <v>10</v>
       </c>
-      <c r="J4" s="2">
+      <c r="L4" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -637,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -649,12 +682,18 @@
         <v>0</v>
       </c>
       <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -666,27 +705,33 @@
         <v>20</v>
       </c>
       <c r="E6" s="2">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2">
+        <v>38</v>
+      </c>
+      <c r="G6" s="2">
         <v>2</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
         <v>9</v>
       </c>
-      <c r="H6" s="2">
+      <c r="J6" s="2">
         <v>6</v>
       </c>
-      <c r="I6" s="2">
+      <c r="K6" s="2">
         <v>11</v>
       </c>
-      <c r="J6" s="2">
+      <c r="L6" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -698,21 +743,27 @@
         <v>11</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
         <v>16</v>
       </c>
-      <c r="H7" s="2">
+      <c r="J7" s="2">
         <v>2</v>
       </c>
-      <c r="I7" s="2">
+      <c r="K7" s="2">
         <v>13</v>
       </c>
-      <c r="J7" s="2">
+      <c r="L7" s="2">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added author labels to the reports
</commit_message>
<xml_diff>
--- a/Python/Data/Final/summary.xlsx
+++ b/Python/Data/Final/summary.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\IUB\CNS_parttime\ASCTB Azimuth Comparison\ASCTB-Azimuth-Comparison-22\Python\Data\Final\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5885E7D-5FD4-4AEC-A738-77CE156ABB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -85,8 +79,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,14 +143,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -203,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,27 +221,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,24 +255,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,32 +430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.5546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,12 +481,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>43</v>
@@ -563,16 +495,16 @@
         <v>64</v>
       </c>
       <c r="E2">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F2">
-        <v>58.139534883720927</v>
+        <v>104.6511627906977</v>
       </c>
       <c r="G2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2">
-        <v>34.375</v>
+        <v>37.5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -584,21 +516,21 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N2">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -616,7 +548,7 @@
         <v>12</v>
       </c>
       <c r="H3">
-        <v>46.153846153846153</v>
+        <v>46.15384615384615</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -628,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -637,12 +569,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>42</v>
@@ -651,16 +583,16 @@
         <v>47</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>33.333333333333343</v>
+        <v>40.47619047619047</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4">
-        <v>21.276595744680851</v>
+        <v>23.40425531914894</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -672,16 +604,16 @@
         <v>7</v>
       </c>
       <c r="L4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N4">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -695,10 +627,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>189</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>1890</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -713,10 +645,10 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -725,12 +657,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>38</v>
@@ -742,25 +674,25 @@
         <v>9</v>
       </c>
       <c r="F6">
-        <v>23.684210526315791</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>35.13513513513514</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>8</v>
+      </c>
+      <c r="L6">
         <v>11</v>
-      </c>
-      <c r="H6">
-        <v>29.72972972972973</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
       </c>
       <c r="M6">
         <v>9</v>
@@ -769,12 +701,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>36</v>
@@ -783,16 +715,16 @@
         <v>26</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>25</v>
+        <v>33.33333333333334</v>
       </c>
       <c r="G7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7">
-        <v>50</v>
+        <v>53.84615384615385</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -801,13 +733,13 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M7">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="N7">
         <v>2</v>

</xml_diff>

<commit_message>
Added changes too code to fix unique CT counts
</commit_message>
<xml_diff>
--- a/Python/Data/Final/summary.xlsx
+++ b/Python/Data/Final/summary.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\IUB\CNS_parttime\ASCTB Azimuth Comparison\ASCTB-Azimuth-Comparison-22\Python\Data\Final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EB755E-21DD-4C64-A8BD-9E2B84582A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -31,13 +37,13 @@
     <t>Az_cts_not_matched</t>
   </si>
   <si>
-    <t>Az_percent_not_matching(%)</t>
+    <t>Az_pecentage_not_matched</t>
   </si>
   <si>
     <t>Asctb_cts_not_matched</t>
   </si>
   <si>
-    <t>Asctb_percent_not_matching(%)</t>
+    <t>Asctb_percentage_not_matched</t>
   </si>
   <si>
     <t>Az_missing_cts</t>
@@ -79,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +149,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -189,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,9 +235,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -255,6 +287,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,14 +480,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +549,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -489,22 +557,22 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="D2">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="E2">
         <v>45</v>
       </c>
       <c r="F2">
-        <v>104.6511627906977</v>
+        <v>67.164179104477611</v>
       </c>
       <c r="G2">
         <v>24</v>
       </c>
       <c r="H2">
-        <v>37.5</v>
+        <v>23.52941176470588</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -525,7 +593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -533,22 +601,22 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3">
-        <v>25</v>
+        <v>23.07692307692308</v>
       </c>
       <c r="G3">
         <v>12</v>
       </c>
       <c r="H3">
-        <v>46.15384615384615</v>
+        <v>37.5</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -569,7 +637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -577,22 +645,22 @@
         <v>36</v>
       </c>
       <c r="C4">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="D4">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E4">
         <v>17</v>
       </c>
       <c r="F4">
-        <v>40.47619047619047</v>
+        <v>26.984126984126981</v>
       </c>
       <c r="G4">
         <v>11</v>
       </c>
       <c r="H4">
-        <v>23.40425531914894</v>
+        <v>17.460317460317459</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -613,7 +681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -621,16 +689,16 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>190</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="E5">
         <v>189</v>
       </c>
       <c r="F5">
-        <v>1890</v>
+        <v>99.473684210526315</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -657,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -665,22 +733,22 @@
         <v>32</v>
       </c>
       <c r="C6">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D6">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="E6">
         <v>9</v>
       </c>
       <c r="F6">
-        <v>23.68421052631579</v>
+        <v>18.367346938775508</v>
       </c>
       <c r="G6">
         <v>13</v>
       </c>
       <c r="H6">
-        <v>35.13513513513514</v>
+        <v>23.63636363636364</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -701,7 +769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -709,22 +777,22 @@
         <v>29</v>
       </c>
       <c r="C7">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="D7">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>12</v>
       </c>
       <c r="F7">
-        <v>33.33333333333334</v>
+        <v>15.38461538461539</v>
       </c>
       <c r="G7">
         <v>14</v>
       </c>
       <c r="H7">
-        <v>53.84615384615385</v>
+        <v>43.75</v>
       </c>
       <c r="I7">
         <v>0</v>

</xml_diff>